<commit_message>
jo kann verwendet werden. Es fehlen noch Bibelverse, aber für den Ablauf und Gebete .... läuft
</commit_message>
<xml_diff>
--- a/Infoinput.xlsx
+++ b/Infoinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyrian\github\Aaron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2E8105-9D4C-45FE-993E-97F07D6A5887}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ACB3D7-C009-4B55-B26E-9020F214D634}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Ort der Bestattung</t>
   </si>
   <si>
-    <t>Sarg</t>
-  </si>
-  <si>
     <t>Garten</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>"Viertes Lied"</t>
+  </si>
+  <si>
+    <t>der Sarg</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="B1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +511,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -566,47 +566,47 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +618,7 @@
       <formula1>"Weg,Säulen,Bild,Psalm23,Freude"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{9BDD0248-09D6-4BA8-9EC9-9AA9628DAF5D}">
-      <formula1>"Urne,Sarg"</formula1>
+      <formula1>"die Urne,der Sarg"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{0A22D034-136A-41EE-B135-C32D757F39A9}">
       <formula1>"Friedhof,Waldfriedhof,Kolumbarium,NurGrab"</formula1>

</xml_diff>

<commit_message>
Personal- und Possesivpronomen eingefügt für feminine und maskuline Anredeformen ... Hab endlich verstanden wie das mit den Pronomen funktioniert ... sehr nice.
</commit_message>
<xml_diff>
--- a/Infoinput.xlsx
+++ b/Infoinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyrian\github\Aaron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ACB3D7-C009-4B55-B26E-9020F214D634}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835E9873-E827-4CDA-9935-60FC825F8EE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Geschlecht</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Geburtsdatum</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>der Sarg</t>
+  </si>
+  <si>
+    <t>weiblich</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="B1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,12 +481,12 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>32031</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>44274</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <f>DATEDIF(C4,C5,"Y")</f>
@@ -511,15 +511,15 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -527,51 +527,51 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -579,38 +579,38 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C14" xr:uid="{6A24A58D-30D0-4DBA-B39A-F56327315FE0}">
       <formula1>"Familie,Ehe,Urlaub,Hobby,Garten,Glaube"</formula1>
     </dataValidation>
@@ -626,6 +626,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27" xr:uid="{C1190F82-13BA-4C14-AD7D-83BC2084AD55}">
       <formula1>"2,3,4,"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{4DA9E19E-C903-4DF6-8188-317ACA46697E}">
+      <formula1>"männlich,weiblich"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Artikel bei Bestattungsform ergänzt
</commit_message>
<xml_diff>
--- a/Infoinput.xlsx
+++ b/Infoinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyrian\github\Aaron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EED53A-A754-4BB0-A6D7-3CE74CBA6DB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD305FB6-BAAA-45C1-9210-F5CED70751C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,13 +120,13 @@
     <t>"Viertes Lied"</t>
   </si>
   <si>
-    <t>der Sarg</t>
-  </si>
-  <si>
     <t>weiblich</t>
   </si>
   <si>
     <t>Psalm23</t>
+  </si>
+  <si>
+    <t>Urne</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
       <formula1>"Weg,Säulen,Bild,Psalm23,Freude"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{9BDD0248-09D6-4BA8-9EC9-9AA9628DAF5D}">
-      <formula1>"die Urne,der Sarg"</formula1>
+      <formula1>"Urne,Sarg"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{0A22D034-136A-41EE-B135-C32D757F39A9}">
       <formula1>"Friedhof,Waldfriedhof,Kolumbarium,NurGrab"</formula1>

</xml_diff>

<commit_message>
Veränderungen in den Bricks: Bild und Regenbogen hinzugefügt bei den Ansprachen
</commit_message>
<xml_diff>
--- a/Infoinput.xlsx
+++ b/Infoinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Dörr\PycharmProjects\Aaron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CB85C2-7070-4288-944A-280B605EC59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A12D0C-0BDC-408C-87D1-F948F872ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>